<commit_message>
deleted old tester, added objective value print
</commit_message>
<xml_diff>
--- a/results/scheduleraw.xlsx.xlsx
+++ b/results/scheduleraw.xlsx.xlsx
@@ -1,33 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe753deea9fa81e/Documents/GitHub/Strathdar/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_36118080FA576A5EB80B8DB0FB2D62B1A0BBDC62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EE5AB62-F2DC-48F2-9C1D-714A85E9DD11}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -61,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,26 +96,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -180,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,27 +185,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,24 +219,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,16 +394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P301"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="I301" sqref="I301"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -521,7 +456,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -550,7 +485,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -579,7 +514,7 @@
         <v>2700000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -608,7 +543,7 @@
         <v>2610180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -637,7 +572,7 @@
         <v>2520360</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -666,7 +601,7 @@
         <v>2430540</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -695,7 +630,7 @@
         <v>2340720</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -724,7 +659,7 @@
         <v>2250900</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -753,7 +688,7 @@
         <v>2161080</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -782,7 +717,7 @@
         <v>2071260</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -811,7 +746,7 @@
         <v>1981440</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -840,7 +775,7 @@
         <v>1891620</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -869,7 +804,7 @@
         <v>1801800</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -898,7 +833,7 @@
         <v>1711980</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -927,7 +862,7 @@
         <v>1622160</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -956,7 +891,7 @@
         <v>1532340</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -985,7 +920,7 @@
         <v>1442520</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1014,7 +949,7 @@
         <v>1352700</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1043,7 +978,7 @@
         <v>1262880</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1072,7 +1007,7 @@
         <v>2162880</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1101,7 +1036,7 @@
         <v>3062880</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1130,7 +1065,7 @@
         <v>3962880</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1159,7 +1094,7 @@
         <v>4862880</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1188,7 +1123,7 @@
         <v>5762880</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1217,7 +1152,7 @@
         <v>6662880</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1246,7 +1181,7 @@
         <v>7562880</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1275,7 +1210,7 @@
         <v>8462880</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1304,7 +1239,7 @@
         <v>9362880</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1333,7 +1268,7 @@
         <v>10262880</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1362,7 +1297,7 @@
         <v>11162880</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1391,7 +1326,7 @@
         <v>12062880</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1420,7 +1355,7 @@
         <v>11973060</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1449,7 +1384,7 @@
         <v>11883240</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1478,7 +1413,7 @@
         <v>11793420</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1507,7 +1442,7 @@
         <v>11703600</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1536,7 +1471,7 @@
         <v>11613780</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1565,7 +1500,7 @@
         <v>11523960</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1594,7 +1529,7 @@
         <v>11434140</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1623,7 +1558,7 @@
         <v>11344320</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1652,7 +1587,7 @@
         <v>11342412</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1681,7 +1616,7 @@
         <v>11252592</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1710,7 +1645,7 @@
         <v>11162772</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1739,7 +1674,7 @@
         <v>11072952</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1768,7 +1703,7 @@
         <v>10983132</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1797,7 +1732,7 @@
         <v>10893312</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1826,7 +1761,7 @@
         <v>10803492</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1855,7 +1790,7 @@
         <v>11703492</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1884,7 +1819,7 @@
         <v>12603492</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1913,7 +1848,7 @@
         <v>12513672</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1942,7 +1877,7 @@
         <v>12423852</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1971,7 +1906,7 @@
         <v>12334032</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2000,7 +1935,7 @@
         <v>12244212</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2028,26 +1963,8 @@
       <c r="I54">
         <v>12154392</v>
       </c>
-      <c r="L54">
-        <v>150</v>
-      </c>
-      <c r="M54">
-        <f>F54*L54</f>
-        <v>12150000</v>
-      </c>
-      <c r="N54">
-        <v>0.3</v>
-      </c>
-      <c r="O54">
-        <f>N54*G54</f>
-        <v>4392</v>
-      </c>
-      <c r="P54">
-        <f>M54+O54</f>
-        <v>12154392</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2075,14 +1992,8 @@
       <c r="I55">
         <v>12154392</v>
       </c>
-      <c r="L55">
-        <v>150</v>
-      </c>
-      <c r="N55">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2110,14 +2021,8 @@
       <c r="I56">
         <v>13054392</v>
       </c>
-      <c r="L56">
-        <v>150</v>
-      </c>
-      <c r="N56">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2145,14 +2050,8 @@
       <c r="I57">
         <v>13954392</v>
       </c>
-      <c r="L57">
-        <v>150</v>
-      </c>
-      <c r="N57">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2180,14 +2079,8 @@
       <c r="I58">
         <v>14854392</v>
       </c>
-      <c r="L58">
-        <v>150</v>
-      </c>
-      <c r="N58">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2215,14 +2108,8 @@
       <c r="I59">
         <v>15754392</v>
       </c>
-      <c r="L59">
-        <v>150</v>
-      </c>
-      <c r="N59">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2250,14 +2137,8 @@
       <c r="I60">
         <v>16654392</v>
       </c>
-      <c r="L60">
-        <v>150</v>
-      </c>
-      <c r="N60">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2285,11 +2166,8 @@
       <c r="I61">
         <v>17554392</v>
       </c>
-      <c r="L61">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2317,11 +2195,8 @@
       <c r="I62">
         <v>18454392</v>
       </c>
-      <c r="L62">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2349,11 +2224,8 @@
       <c r="I63">
         <v>19354392</v>
       </c>
-      <c r="L63">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2381,11 +2253,8 @@
       <c r="I64">
         <v>20254392</v>
       </c>
-      <c r="L64">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2413,11 +2282,8 @@
       <c r="I65">
         <v>21154392</v>
       </c>
-      <c r="L65">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2445,11 +2311,8 @@
       <c r="I66">
         <v>22054392</v>
       </c>
-      <c r="L66">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2477,11 +2340,8 @@
       <c r="I67">
         <v>21964572</v>
       </c>
-      <c r="L67">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2509,11 +2369,8 @@
       <c r="I68">
         <v>21874752</v>
       </c>
-      <c r="L68">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2541,11 +2398,8 @@
       <c r="I69">
         <v>21784932</v>
       </c>
-      <c r="L69">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2573,11 +2427,8 @@
       <c r="I70">
         <v>21695112</v>
       </c>
-      <c r="L70">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2605,11 +2456,8 @@
       <c r="I71">
         <v>21605292</v>
       </c>
-      <c r="L71">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2637,11 +2485,8 @@
       <c r="I72">
         <v>21515472</v>
       </c>
-      <c r="L72">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2669,11 +2514,8 @@
       <c r="I73">
         <v>21425652</v>
       </c>
-      <c r="L73">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2701,11 +2543,8 @@
       <c r="I74">
         <v>21335832</v>
       </c>
-      <c r="L74">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2733,11 +2572,8 @@
       <c r="I75">
         <v>21246012</v>
       </c>
-      <c r="L75">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2765,11 +2601,8 @@
       <c r="I76">
         <v>21156192</v>
       </c>
-      <c r="L76">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2797,11 +2630,8 @@
       <c r="I77">
         <v>21066372</v>
       </c>
-      <c r="L77">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2829,11 +2659,8 @@
       <c r="I78">
         <v>20976552</v>
       </c>
-      <c r="L78">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2861,11 +2688,8 @@
       <c r="I79">
         <v>20886732</v>
       </c>
-      <c r="L79">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2893,11 +2717,8 @@
       <c r="I80">
         <v>20796912</v>
       </c>
-      <c r="L80">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2925,11 +2746,8 @@
       <c r="I81">
         <v>20707092</v>
       </c>
-      <c r="L81">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2957,11 +2775,8 @@
       <c r="I82">
         <v>20617272</v>
       </c>
-      <c r="L82">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2989,11 +2804,8 @@
       <c r="I83">
         <v>20527452</v>
       </c>
-      <c r="L83">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3021,11 +2833,8 @@
       <c r="I84">
         <v>20437632</v>
       </c>
-      <c r="L84">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3053,11 +2862,8 @@
       <c r="I85">
         <v>20347812</v>
       </c>
-      <c r="L85">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3085,11 +2891,8 @@
       <c r="I86">
         <v>20257992</v>
       </c>
-      <c r="L86">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3117,11 +2920,8 @@
       <c r="I87">
         <v>20168172</v>
       </c>
-      <c r="L87">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3149,11 +2949,8 @@
       <c r="I88">
         <v>20078352</v>
       </c>
-      <c r="L88">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3181,11 +2978,8 @@
       <c r="I89">
         <v>19988532</v>
       </c>
-      <c r="L89">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3213,11 +3007,8 @@
       <c r="I90">
         <v>19898712</v>
       </c>
-      <c r="L90">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3245,11 +3036,8 @@
       <c r="I91">
         <v>19808892</v>
       </c>
-      <c r="L91">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3277,11 +3065,8 @@
       <c r="I92">
         <v>19719072</v>
       </c>
-      <c r="L92">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3309,11 +3094,8 @@
       <c r="I93">
         <v>20619072</v>
       </c>
-      <c r="L93">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3341,11 +3123,8 @@
       <c r="I94">
         <v>20619072</v>
       </c>
-      <c r="L94">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3373,11 +3152,8 @@
       <c r="I95">
         <v>21519072</v>
       </c>
-      <c r="L95">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3405,11 +3181,8 @@
       <c r="I96">
         <v>22419072</v>
       </c>
-      <c r="L96">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3437,11 +3210,8 @@
       <c r="I97">
         <v>23319072</v>
       </c>
-      <c r="L97">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3470,7 +3240,7 @@
         <v>23229252</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3499,7 +3269,7 @@
         <v>23139432</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3528,7 +3298,7 @@
         <v>23049612</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3557,7 +3327,7 @@
         <v>22959792</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3586,7 +3356,7 @@
         <v>22869972</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3615,7 +3385,7 @@
         <v>22780152</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3644,7 +3414,7 @@
         <v>22690332</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3673,7 +3443,7 @@
         <v>22600512</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3702,7 +3472,7 @@
         <v>22510692</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3731,7 +3501,7 @@
         <v>22420872</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3760,7 +3530,7 @@
         <v>22331052</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3789,7 +3559,7 @@
         <v>22241232</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3818,7 +3588,7 @@
         <v>22151412</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3847,7 +3617,7 @@
         <v>22061592</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3876,7 +3646,7 @@
         <v>21971772</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3905,7 +3675,7 @@
         <v>21881952</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3934,7 +3704,7 @@
         <v>21792132</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3963,7 +3733,7 @@
         <v>21702312</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3992,7 +3762,7 @@
         <v>21612492</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4021,7 +3791,7 @@
         <v>21522672</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4050,7 +3820,7 @@
         <v>21432852</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4079,7 +3849,7 @@
         <v>21343032</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4108,7 +3878,7 @@
         <v>21253212</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4137,7 +3907,7 @@
         <v>21163392</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4166,7 +3936,7 @@
         <v>21073572</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4195,7 +3965,7 @@
         <v>20983752</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4224,7 +3994,7 @@
         <v>20893932</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4253,7 +4023,7 @@
         <v>20804112</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4282,7 +4052,7 @@
         <v>20714292</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4311,7 +4081,7 @@
         <v>20624472</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4340,7 +4110,7 @@
         <v>20534652</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4369,7 +4139,7 @@
         <v>20444832</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4398,7 +4168,7 @@
         <v>20355012</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4427,7 +4197,7 @@
         <v>20265192</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4456,7 +4226,7 @@
         <v>20175372</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4485,7 +4255,7 @@
         <v>20085552</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4514,7 +4284,7 @@
         <v>19995732</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4543,7 +4313,7 @@
         <v>20895732</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4572,7 +4342,7 @@
         <v>21795732</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4601,7 +4371,7 @@
         <v>22695732</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4630,7 +4400,7 @@
         <v>23595732</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4659,7 +4429,7 @@
         <v>24495732</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4688,7 +4458,7 @@
         <v>25395732</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4717,7 +4487,7 @@
         <v>26295732</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4746,7 +4516,7 @@
         <v>27195732</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4775,7 +4545,7 @@
         <v>28095732</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4804,7 +4574,7 @@
         <v>28995732</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4833,7 +4603,7 @@
         <v>29895732</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4862,7 +4632,7 @@
         <v>29805912</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4891,7 +4661,7 @@
         <v>29716092</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4920,7 +4690,7 @@
         <v>29626272</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4949,7 +4719,7 @@
         <v>29536452</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4978,7 +4748,7 @@
         <v>29446632</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5007,7 +4777,7 @@
         <v>29356812</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5036,7 +4806,7 @@
         <v>29266992</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5065,7 +4835,7 @@
         <v>29177172</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5094,7 +4864,7 @@
         <v>29087352</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5123,7 +4893,7 @@
         <v>28997532</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5152,7 +4922,7 @@
         <v>28907712</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5181,7 +4951,7 @@
         <v>28817892</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5210,7 +4980,7 @@
         <v>28728072</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5239,7 +5009,7 @@
         <v>28638252</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5268,7 +5038,7 @@
         <v>28548432</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5297,7 +5067,7 @@
         <v>28458612</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5326,7 +5096,7 @@
         <v>28368792</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5355,7 +5125,7 @@
         <v>28278972</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5384,7 +5154,7 @@
         <v>28189152</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5413,7 +5183,7 @@
         <v>28099332</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5442,7 +5212,7 @@
         <v>28009512</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5471,7 +5241,7 @@
         <v>27919692</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -5500,7 +5270,7 @@
         <v>28819692</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -5529,7 +5299,7 @@
         <v>29719692</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -5558,7 +5328,7 @@
         <v>30619692</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -5587,7 +5357,7 @@
         <v>31519692</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -5616,7 +5386,7 @@
         <v>32419692</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -5645,7 +5415,7 @@
         <v>33319692</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -5674,7 +5444,7 @@
         <v>34219692</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -5703,7 +5473,7 @@
         <v>35119692</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -5732,7 +5502,7 @@
         <v>36019692</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -5761,7 +5531,7 @@
         <v>36919692</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -5790,7 +5560,7 @@
         <v>37819692</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -5819,7 +5589,7 @@
         <v>38719692</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5848,7 +5618,7 @@
         <v>38629872</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -5877,7 +5647,7 @@
         <v>38540052</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -5906,7 +5676,7 @@
         <v>38450232</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -5935,7 +5705,7 @@
         <v>38360412</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -5964,7 +5734,7 @@
         <v>38270592</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -5993,7 +5763,7 @@
         <v>38180772</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6022,7 +5792,7 @@
         <v>39080772</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6051,7 +5821,7 @@
         <v>39980772</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6080,7 +5850,7 @@
         <v>40880772</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6109,7 +5879,7 @@
         <v>41780772</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6138,7 +5908,7 @@
         <v>42680772</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6167,7 +5937,7 @@
         <v>43580772</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6196,7 +5966,7 @@
         <v>43490952</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6225,7 +5995,7 @@
         <v>43401132</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6254,7 +6024,7 @@
         <v>43311312</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6283,7 +6053,7 @@
         <v>43221492</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6312,7 +6082,7 @@
         <v>43131672</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6341,7 +6111,7 @@
         <v>43041852</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -6370,7 +6140,7 @@
         <v>42952032</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -6399,7 +6169,7 @@
         <v>42862212</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -6428,7 +6198,7 @@
         <v>42772392</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -6457,7 +6227,7 @@
         <v>42682572</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -6486,7 +6256,7 @@
         <v>42592752</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -6515,7 +6285,7 @@
         <v>42502932</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -6544,7 +6314,7 @@
         <v>42413112</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -6573,7 +6343,7 @@
         <v>42323292</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -6602,7 +6372,7 @@
         <v>42233472</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -6631,7 +6401,7 @@
         <v>42143652</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -6660,7 +6430,7 @@
         <v>42053832</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -6689,7 +6459,7 @@
         <v>41964012</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -6718,7 +6488,7 @@
         <v>41874192</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -6747,7 +6517,7 @@
         <v>41784372</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -6776,7 +6546,7 @@
         <v>41694552</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -6805,7 +6575,7 @@
         <v>41604732</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -6834,7 +6604,7 @@
         <v>41514912</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -6863,7 +6633,7 @@
         <v>41425092</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -6892,7 +6662,7 @@
         <v>41335272</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -6921,7 +6691,7 @@
         <v>41245452</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -6950,7 +6720,7 @@
         <v>41155632</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -6979,7 +6749,7 @@
         <v>41065812</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -7008,7 +6778,7 @@
         <v>40975992</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -7037,7 +6807,7 @@
         <v>40886172</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -7066,7 +6836,7 @@
         <v>40796352</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -7095,7 +6865,7 @@
         <v>40706532</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -7124,7 +6894,7 @@
         <v>40616712</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -7153,7 +6923,7 @@
         <v>40526892</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -7182,7 +6952,7 @@
         <v>40437072</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -7211,7 +6981,7 @@
         <v>40347252</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -7240,7 +7010,7 @@
         <v>40257432</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -7269,7 +7039,7 @@
         <v>40167612</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -7298,7 +7068,7 @@
         <v>40077792</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -7327,7 +7097,7 @@
         <v>39987972</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -7356,7 +7126,7 @@
         <v>40887972</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -7385,7 +7155,7 @@
         <v>41787972</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -7414,7 +7184,7 @@
         <v>42687972</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -7443,7 +7213,7 @@
         <v>43587972</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -7472,7 +7242,7 @@
         <v>44487972</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -7501,7 +7271,7 @@
         <v>44398152</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -7530,7 +7300,7 @@
         <v>44308332</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -7559,7 +7329,7 @@
         <v>44308332</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -7588,7 +7358,7 @@
         <v>44308332</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -7617,7 +7387,7 @@
         <v>44218512</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -7646,7 +7416,7 @@
         <v>44128692</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -7675,7 +7445,7 @@
         <v>44038872</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -7704,7 +7474,7 @@
         <v>44038872</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -7733,7 +7503,7 @@
         <v>43949052</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -7762,7 +7532,7 @@
         <v>43859232</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -7791,7 +7561,7 @@
         <v>43769412</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -7820,7 +7590,7 @@
         <v>44669412</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -7849,7 +7619,7 @@
         <v>45569412</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -7878,7 +7648,7 @@
         <v>46469412</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -7907,7 +7677,7 @@
         <v>47369412</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -7936,7 +7706,7 @@
         <v>48269412</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -7965,7 +7735,7 @@
         <v>49169412</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -7994,7 +7764,7 @@
         <v>50069412</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -8023,7 +7793,7 @@
         <v>50969412</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -8052,7 +7822,7 @@
         <v>51869412</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -8081,7 +7851,7 @@
         <v>52769412</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -8110,7 +7880,7 @@
         <v>53669412</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -8139,7 +7909,7 @@
         <v>53579592</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -8168,7 +7938,7 @@
         <v>53579592</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -8197,7 +7967,7 @@
         <v>53489772</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -8226,7 +7996,7 @@
         <v>53399952</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -8255,7 +8025,7 @@
         <v>53310132</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -8284,7 +8054,7 @@
         <v>53310132</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -8313,7 +8083,7 @@
         <v>53220312</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -8342,7 +8112,7 @@
         <v>53130492</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -8371,7 +8141,7 @@
         <v>53040672</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -8400,7 +8170,7 @@
         <v>52950852</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -8429,7 +8199,7 @@
         <v>52861032</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -8458,7 +8228,7 @@
         <v>52771212</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -8487,7 +8257,7 @@
         <v>52681392</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -8516,7 +8286,7 @@
         <v>52681392</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -8545,7 +8315,7 @@
         <v>52591572</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -8574,7 +8344,7 @@
         <v>52501752</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -8603,7 +8373,7 @@
         <v>52411932</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -8632,7 +8402,7 @@
         <v>52322112</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -8661,7 +8431,7 @@
         <v>52232292</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -8690,7 +8460,7 @@
         <v>53132292</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -8719,7 +8489,7 @@
         <v>54032292</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -8748,7 +8518,7 @@
         <v>54932292</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -8777,7 +8547,7 @@
         <v>55832292</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -8806,7 +8576,7 @@
         <v>56732292</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -8835,7 +8605,7 @@
         <v>57632292</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -8864,7 +8634,7 @@
         <v>58532292</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -8893,7 +8663,7 @@
         <v>59432292</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -8922,7 +8692,7 @@
         <v>60332292</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -8951,7 +8721,7 @@
         <v>61232292</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -8980,7 +8750,7 @@
         <v>62132292</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -9009,7 +8779,7 @@
         <v>63032292</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -9038,7 +8808,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -9067,7 +8837,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -9096,7 +8866,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -9125,7 +8895,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -9154,7 +8924,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -9183,7 +8953,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -9212,7 +8982,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -9241,7 +9011,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -9270,7 +9040,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -9299,7 +9069,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -9328,7 +9098,7 @@
         <v>63932292</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -9353,7 +9123,7 @@
       <c r="H301">
         <v>6360</v>
       </c>
-      <c r="I301" s="2">
+      <c r="I301">
         <v>63932292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed switching constraint at start/end of time inte
</commit_message>
<xml_diff>
--- a/results/scheduleraw.xlsx.xlsx
+++ b/results/scheduleraw.xlsx.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="she7et1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -447,10 +447,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -459,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>900000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>900000</v>
+        <v>1800000</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>12000</v>
+        <v>18000</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1800000</v>
+        <v>2700000</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>18000</v>
+        <v>24000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2700000</v>
+        <v>3600000</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>17400</v>
+        <v>23400</v>
       </c>
       <c r="G6">
         <v>600</v>
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2610180</v>
+        <v>3510180</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>16800</v>
+        <v>22800</v>
       </c>
       <c r="G7">
         <v>1200</v>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2520360</v>
+        <v>3420360</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>16200</v>
+        <v>22200</v>
       </c>
       <c r="G8">
         <v>1800</v>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2430540</v>
+        <v>3330540</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>15600</v>
+        <v>21600</v>
       </c>
       <c r="G9">
         <v>2400</v>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2340720</v>
+        <v>3240720</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -706,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>15000</v>
+        <v>21000</v>
       </c>
       <c r="G10">
         <v>3000</v>
@@ -715,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2250900</v>
+        <v>3150900</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>14400</v>
+        <v>20400</v>
       </c>
       <c r="G11">
         <v>3600</v>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2161080</v>
+        <v>3061080</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>13800</v>
+        <v>19800</v>
       </c>
       <c r="G12">
         <v>4200</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2071260</v>
+        <v>2971260</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>13200</v>
+        <v>19200</v>
       </c>
       <c r="G13">
         <v>4800</v>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>1981440</v>
+        <v>2881440</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>12600</v>
+        <v>18600</v>
       </c>
       <c r="G14">
         <v>5400</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1891620</v>
+        <v>2791620</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>12000</v>
+        <v>18000</v>
       </c>
       <c r="G15">
         <v>6000</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1801800</v>
+        <v>2701800</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>11400</v>
+        <v>17400</v>
       </c>
       <c r="G16">
         <v>6600</v>
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1711980</v>
+        <v>2611980</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>10800</v>
+        <v>16800</v>
       </c>
       <c r="G17">
         <v>7200</v>
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1622160</v>
+        <v>2522160</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>10200</v>
+        <v>16200</v>
       </c>
       <c r="G18">
         <v>7800</v>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1532340</v>
+        <v>2432340</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>9600</v>
+        <v>15600</v>
       </c>
       <c r="G19">
         <v>8400</v>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1442520</v>
+        <v>2342520</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="G20">
         <v>9000</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1352700</v>
+        <v>2252700</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>8400</v>
+        <v>14400</v>
       </c>
       <c r="G21">
         <v>9600</v>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1262880</v>
+        <v>2162880</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>14400</v>
+        <v>20400</v>
       </c>
       <c r="G22">
         <v>9600</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>2162880</v>
+        <v>3062880</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>20400</v>
+        <v>26400</v>
       </c>
       <c r="G23">
         <v>9600</v>
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>3062880</v>
+        <v>3962880</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1142,7 +1142,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1151,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>20400</v>
+        <v>32400</v>
       </c>
       <c r="G24">
         <v>9600</v>
@@ -1163,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>3062880</v>
+        <v>4862880</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1174,7 +1174,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1183,10 +1183,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>20400</v>
+        <v>38400</v>
       </c>
       <c r="G25">
         <v>9600</v>
@@ -1195,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>3062880</v>
+        <v>5762880</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1206,7 +1206,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>20400</v>
+        <v>44400</v>
       </c>
       <c r="G26">
         <v>9600</v>
@@ -1227,10 +1227,10 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>3062880</v>
+        <v>6662880</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1238,7 +1238,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>20400</v>
+        <v>50400</v>
       </c>
       <c r="G27">
         <v>9600</v>
@@ -1259,10 +1259,10 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>3062880</v>
+        <v>7562880</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1270,7 +1270,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1279,10 +1279,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>20400</v>
+        <v>56400</v>
       </c>
       <c r="G28">
         <v>9600</v>
@@ -1291,10 +1291,10 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>3062880</v>
+        <v>8462880</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1302,7 +1302,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1311,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>20400</v>
+        <v>62400</v>
       </c>
       <c r="G29">
         <v>9600</v>
@@ -1323,10 +1323,10 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>3062880</v>
+        <v>9362880</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1334,7 +1334,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1343,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>20400</v>
+        <v>68400</v>
       </c>
       <c r="G30">
         <v>9600</v>
@@ -1355,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>3062880</v>
+        <v>10262880</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1366,7 +1366,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>20400</v>
+        <v>74400</v>
       </c>
       <c r="G31">
         <v>9600</v>
@@ -1387,9 +1387,2249 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>3062880</v>
+        <v>11162880</v>
       </c>
       <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>73800</v>
+      </c>
+      <c r="G32">
+        <v>10200</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>11073060</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>73200</v>
+      </c>
+      <c r="G33">
+        <v>10800</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>10983240</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>72600</v>
+      </c>
+      <c r="G34">
+        <v>11400</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>10893420</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>72000</v>
+      </c>
+      <c r="G35">
+        <v>12000</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>10803600</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>71400</v>
+      </c>
+      <c r="G36">
+        <v>12600</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>10713780</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>70800</v>
+      </c>
+      <c r="G37">
+        <v>13200</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>10623960</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>70200</v>
+      </c>
+      <c r="G38">
+        <v>13800</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>10534140</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>69600</v>
+      </c>
+      <c r="G39">
+        <v>14400</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>10444320</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>69000</v>
+      </c>
+      <c r="G40">
+        <v>15000</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>10354500</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>69000</v>
+      </c>
+      <c r="G41">
+        <v>8640</v>
+      </c>
+      <c r="H41">
+        <v>6360</v>
+      </c>
+      <c r="I41">
+        <v>10352592</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>69000</v>
+      </c>
+      <c r="G42">
+        <v>2280</v>
+      </c>
+      <c r="H42">
+        <v>12720</v>
+      </c>
+      <c r="I42">
+        <v>10350684</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>75000</v>
+      </c>
+      <c r="G43">
+        <v>2280</v>
+      </c>
+      <c r="H43">
+        <v>12720</v>
+      </c>
+      <c r="I43">
+        <v>11250684</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>81000</v>
+      </c>
+      <c r="G44">
+        <v>2280</v>
+      </c>
+      <c r="H44">
+        <v>12720</v>
+      </c>
+      <c r="I44">
+        <v>12150684</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>87000</v>
+      </c>
+      <c r="G45">
+        <v>2280</v>
+      </c>
+      <c r="H45">
+        <v>12720</v>
+      </c>
+      <c r="I45">
+        <v>13050684</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>93000</v>
+      </c>
+      <c r="G46">
+        <v>2280</v>
+      </c>
+      <c r="H46">
+        <v>12720</v>
+      </c>
+      <c r="I46">
+        <v>13950684</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>99000</v>
+      </c>
+      <c r="G47">
+        <v>2280</v>
+      </c>
+      <c r="H47">
+        <v>12720</v>
+      </c>
+      <c r="I47">
+        <v>14850684</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>99000</v>
+      </c>
+      <c r="G48">
+        <v>2280</v>
+      </c>
+      <c r="H48">
+        <v>12720</v>
+      </c>
+      <c r="I48">
+        <v>14850684</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>105000</v>
+      </c>
+      <c r="G49">
+        <v>2280</v>
+      </c>
+      <c r="H49">
+        <v>12720</v>
+      </c>
+      <c r="I49">
+        <v>15750684</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>111000</v>
+      </c>
+      <c r="G50">
+        <v>2280</v>
+      </c>
+      <c r="H50">
+        <v>12720</v>
+      </c>
+      <c r="I50">
+        <v>16650684</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>111000</v>
+      </c>
+      <c r="G51">
+        <v>2280</v>
+      </c>
+      <c r="H51">
+        <v>12720</v>
+      </c>
+      <c r="I51">
+        <v>16650684</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>117000</v>
+      </c>
+      <c r="G52">
+        <v>2280</v>
+      </c>
+      <c r="H52">
+        <v>12720</v>
+      </c>
+      <c r="I52">
+        <v>17550684</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>123000</v>
+      </c>
+      <c r="G53">
+        <v>2280</v>
+      </c>
+      <c r="H53">
+        <v>12720</v>
+      </c>
+      <c r="I53">
+        <v>18450684</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>129000</v>
+      </c>
+      <c r="G54">
+        <v>2280</v>
+      </c>
+      <c r="H54">
+        <v>12720</v>
+      </c>
+      <c r="I54">
+        <v>19350684</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>135000</v>
+      </c>
+      <c r="G55">
+        <v>2280</v>
+      </c>
+      <c r="H55">
+        <v>12720</v>
+      </c>
+      <c r="I55">
+        <v>20250684</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>141000</v>
+      </c>
+      <c r="G56">
+        <v>2280</v>
+      </c>
+      <c r="H56">
+        <v>12720</v>
+      </c>
+      <c r="I56">
+        <v>21150684</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>147000</v>
+      </c>
+      <c r="G57">
+        <v>2280</v>
+      </c>
+      <c r="H57">
+        <v>12720</v>
+      </c>
+      <c r="I57">
+        <v>22050684</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>153000</v>
+      </c>
+      <c r="G58">
+        <v>2280</v>
+      </c>
+      <c r="H58">
+        <v>12720</v>
+      </c>
+      <c r="I58">
+        <v>22950684</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>159000</v>
+      </c>
+      <c r="G59">
+        <v>2280</v>
+      </c>
+      <c r="H59">
+        <v>12720</v>
+      </c>
+      <c r="I59">
+        <v>23850684</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>165000</v>
+      </c>
+      <c r="G60">
+        <v>2280</v>
+      </c>
+      <c r="H60">
+        <v>12720</v>
+      </c>
+      <c r="I60">
+        <v>24750684</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>171000</v>
+      </c>
+      <c r="G61">
+        <v>2280</v>
+      </c>
+      <c r="H61">
+        <v>12720</v>
+      </c>
+      <c r="I61">
+        <v>25650684</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>177000</v>
+      </c>
+      <c r="G62">
+        <v>2280</v>
+      </c>
+      <c r="H62">
+        <v>12720</v>
+      </c>
+      <c r="I62">
+        <v>26550684</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>183000</v>
+      </c>
+      <c r="G63">
+        <v>2280</v>
+      </c>
+      <c r="H63">
+        <v>12720</v>
+      </c>
+      <c r="I63">
+        <v>27450684</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>189000</v>
+      </c>
+      <c r="G64">
+        <v>2280</v>
+      </c>
+      <c r="H64">
+        <v>12720</v>
+      </c>
+      <c r="I64">
+        <v>28350684</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>195000</v>
+      </c>
+      <c r="G65">
+        <v>2280</v>
+      </c>
+      <c r="H65">
+        <v>12720</v>
+      </c>
+      <c r="I65">
+        <v>29250684</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>201000</v>
+      </c>
+      <c r="G66">
+        <v>2280</v>
+      </c>
+      <c r="H66">
+        <v>12720</v>
+      </c>
+      <c r="I66">
+        <v>30150684</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>207000</v>
+      </c>
+      <c r="G67">
+        <v>2280</v>
+      </c>
+      <c r="H67">
+        <v>12720</v>
+      </c>
+      <c r="I67">
+        <v>31050684</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>207000</v>
+      </c>
+      <c r="G68">
+        <v>2280</v>
+      </c>
+      <c r="H68">
+        <v>12720</v>
+      </c>
+      <c r="I68">
+        <v>31050684</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>207000</v>
+      </c>
+      <c r="G69">
+        <v>2280</v>
+      </c>
+      <c r="H69">
+        <v>12720</v>
+      </c>
+      <c r="I69">
+        <v>31050684</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>207000</v>
+      </c>
+      <c r="G70">
+        <v>2280</v>
+      </c>
+      <c r="H70">
+        <v>12720</v>
+      </c>
+      <c r="I70">
+        <v>31050684</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>207000</v>
+      </c>
+      <c r="G71">
+        <v>2280</v>
+      </c>
+      <c r="H71">
+        <v>12720</v>
+      </c>
+      <c r="I71">
+        <v>31050684</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>207000</v>
+      </c>
+      <c r="G72">
+        <v>2280</v>
+      </c>
+      <c r="H72">
+        <v>12720</v>
+      </c>
+      <c r="I72">
+        <v>31050684</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>207000</v>
+      </c>
+      <c r="G73">
+        <v>2280</v>
+      </c>
+      <c r="H73">
+        <v>12720</v>
+      </c>
+      <c r="I73">
+        <v>31050684</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>207000</v>
+      </c>
+      <c r="G74">
+        <v>2280</v>
+      </c>
+      <c r="H74">
+        <v>12720</v>
+      </c>
+      <c r="I74">
+        <v>31050684</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>207000</v>
+      </c>
+      <c r="G75">
+        <v>2280</v>
+      </c>
+      <c r="H75">
+        <v>12720</v>
+      </c>
+      <c r="I75">
+        <v>31050684</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>207000</v>
+      </c>
+      <c r="G76">
+        <v>2280</v>
+      </c>
+      <c r="H76">
+        <v>12720</v>
+      </c>
+      <c r="I76">
+        <v>31050684</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>207000</v>
+      </c>
+      <c r="G77">
+        <v>2280</v>
+      </c>
+      <c r="H77">
+        <v>12720</v>
+      </c>
+      <c r="I77">
+        <v>31050684</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>207000</v>
+      </c>
+      <c r="G78">
+        <v>2280</v>
+      </c>
+      <c r="H78">
+        <v>12720</v>
+      </c>
+      <c r="I78">
+        <v>31050684</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>207000</v>
+      </c>
+      <c r="G79">
+        <v>2280</v>
+      </c>
+      <c r="H79">
+        <v>12720</v>
+      </c>
+      <c r="I79">
+        <v>31050684</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>207000</v>
+      </c>
+      <c r="G80">
+        <v>2280</v>
+      </c>
+      <c r="H80">
+        <v>12720</v>
+      </c>
+      <c r="I80">
+        <v>31050684</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>207000</v>
+      </c>
+      <c r="G81">
+        <v>2280</v>
+      </c>
+      <c r="H81">
+        <v>12720</v>
+      </c>
+      <c r="I81">
+        <v>31050684</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>207000</v>
+      </c>
+      <c r="G82">
+        <v>2280</v>
+      </c>
+      <c r="H82">
+        <v>12720</v>
+      </c>
+      <c r="I82">
+        <v>31050684</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>207000</v>
+      </c>
+      <c r="G83">
+        <v>2280</v>
+      </c>
+      <c r="H83">
+        <v>12720</v>
+      </c>
+      <c r="I83">
+        <v>31050684</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>207000</v>
+      </c>
+      <c r="G84">
+        <v>2280</v>
+      </c>
+      <c r="H84">
+        <v>12720</v>
+      </c>
+      <c r="I84">
+        <v>31050684</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>207000</v>
+      </c>
+      <c r="G85">
+        <v>2280</v>
+      </c>
+      <c r="H85">
+        <v>12720</v>
+      </c>
+      <c r="I85">
+        <v>31050684</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>207000</v>
+      </c>
+      <c r="G86">
+        <v>2280</v>
+      </c>
+      <c r="H86">
+        <v>12720</v>
+      </c>
+      <c r="I86">
+        <v>31050684</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>207000</v>
+      </c>
+      <c r="G87">
+        <v>2280</v>
+      </c>
+      <c r="H87">
+        <v>12720</v>
+      </c>
+      <c r="I87">
+        <v>31050684</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>207000</v>
+      </c>
+      <c r="G88">
+        <v>2280</v>
+      </c>
+      <c r="H88">
+        <v>12720</v>
+      </c>
+      <c r="I88">
+        <v>31050684</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>207000</v>
+      </c>
+      <c r="G89">
+        <v>2280</v>
+      </c>
+      <c r="H89">
+        <v>12720</v>
+      </c>
+      <c r="I89">
+        <v>31050684</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>207000</v>
+      </c>
+      <c r="G90">
+        <v>2280</v>
+      </c>
+      <c r="H90">
+        <v>12720</v>
+      </c>
+      <c r="I90">
+        <v>31050684</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>207000</v>
+      </c>
+      <c r="G91">
+        <v>2280</v>
+      </c>
+      <c r="H91">
+        <v>12720</v>
+      </c>
+      <c r="I91">
+        <v>31050684</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>207000</v>
+      </c>
+      <c r="G92">
+        <v>2280</v>
+      </c>
+      <c r="H92">
+        <v>12720</v>
+      </c>
+      <c r="I92">
+        <v>31050684</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>207000</v>
+      </c>
+      <c r="G93">
+        <v>2280</v>
+      </c>
+      <c r="H93">
+        <v>12720</v>
+      </c>
+      <c r="I93">
+        <v>31050684</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>213000</v>
+      </c>
+      <c r="G94">
+        <v>2280</v>
+      </c>
+      <c r="H94">
+        <v>12720</v>
+      </c>
+      <c r="I94">
+        <v>31950684</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>219000</v>
+      </c>
+      <c r="G95">
+        <v>2280</v>
+      </c>
+      <c r="H95">
+        <v>12720</v>
+      </c>
+      <c r="I95">
+        <v>32850684</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>225000</v>
+      </c>
+      <c r="G96">
+        <v>2280</v>
+      </c>
+      <c r="H96">
+        <v>12720</v>
+      </c>
+      <c r="I96">
+        <v>33750684</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>231000</v>
+      </c>
+      <c r="G97">
+        <v>2280</v>
+      </c>
+      <c r="H97">
+        <v>12720</v>
+      </c>
+      <c r="I97">
+        <v>34650684</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>231000</v>
+      </c>
+      <c r="G98">
+        <v>2280</v>
+      </c>
+      <c r="H98">
+        <v>12720</v>
+      </c>
+      <c r="I98">
+        <v>34650684</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>231000</v>
+      </c>
+      <c r="G99">
+        <v>2280</v>
+      </c>
+      <c r="H99">
+        <v>12720</v>
+      </c>
+      <c r="I99">
+        <v>34650684</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>231000</v>
+      </c>
+      <c r="G100">
+        <v>2280</v>
+      </c>
+      <c r="H100">
+        <v>12720</v>
+      </c>
+      <c r="I100">
+        <v>34650684</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>231000</v>
+      </c>
+      <c r="G101">
+        <v>2280</v>
+      </c>
+      <c r="H101">
+        <v>12720</v>
+      </c>
+      <c r="I101">
+        <v>34650684</v>
+      </c>
+      <c r="J101">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed issue with write out
still need to check issues with bounderies at intervals
</commit_message>
<xml_diff>
--- a/results/scheduleraw.xlsx.xlsx
+++ b/results/scheduleraw.xlsx.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iainh\Documents\GitHub\Strathdar\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE2214A-4C09-40B0-A521-723790E8C1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="she7et1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -46,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -156,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +202,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +254,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,14 +447,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -465,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -529,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -561,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -593,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -625,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -657,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -689,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -721,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -753,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -785,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -817,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -849,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -881,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -913,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -945,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -977,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1009,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1041,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1073,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1105,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1137,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1169,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1201,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1233,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1265,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1297,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1329,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1361,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1393,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1425,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1457,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1489,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1521,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1553,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1585,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1617,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1649,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1681,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1713,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1745,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1777,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1809,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1841,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1873,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1905,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1937,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1969,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2001,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2033,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2065,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2097,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2129,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2161,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2193,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2225,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2257,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2289,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2321,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2353,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2385,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2417,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2449,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2481,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2513,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2545,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2577,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2609,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2641,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2673,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2705,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2737,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2769,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2801,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2833,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2865,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2897,7 +2949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2929,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2961,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2993,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3025,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3057,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3089,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3121,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3153,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3185,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3217,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3249,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3281,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3313,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3345,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3377,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3409,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3441,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3473,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3505,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3537,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3569,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3601,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3633,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3665,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3697,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3729,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3761,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3793,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3825,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3857,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3889,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3921,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3953,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3985,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4017,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4049,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4081,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4113,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4145,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4177,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4209,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4241,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4273,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4305,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4337,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4369,7 +4421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4401,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4433,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4465,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4497,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4529,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4561,7 +4613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4593,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4625,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4657,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4689,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4721,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4753,7 +4805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4785,7 +4837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4817,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4849,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4881,7 +4933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4913,7 +4965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4945,7 +4997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4977,7 +5029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5009,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5041,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5073,7 +5125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5105,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5137,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5169,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5201,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5233,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5265,7 +5317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5297,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5329,7 +5381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5361,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5393,7 +5445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5425,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5457,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5489,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5521,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5553,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5585,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5617,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5649,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5681,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5713,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5745,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -5777,7 +5829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -5809,7 +5861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -5841,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -5873,7 +5925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -5905,7 +5957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -5937,7 +5989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -5969,7 +6021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6001,7 +6053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6033,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6065,7 +6117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6097,7 +6149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6129,7 +6181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6161,7 +6213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6193,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6225,7 +6277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6257,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6289,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6321,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6353,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6385,7 +6437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6417,7 +6469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6449,7 +6501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6481,7 +6533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6513,7 +6565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6545,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6577,7 +6629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6609,7 +6661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6641,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6673,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6705,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -6737,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -6769,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -6801,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -6833,7 +6885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -6865,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -6897,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -6929,7 +6981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -6961,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -6993,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -7025,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7057,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -7089,7 +7141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -7121,7 +7173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -7153,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -7185,7 +7237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7217,7 +7269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -7249,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -7281,7 +7333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -7313,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -7345,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -7377,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -7409,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -7441,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -7473,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -7505,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -7537,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -7569,7 +7621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -7601,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -7633,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -7665,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -7697,7 +7749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -7729,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -7761,7 +7813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -7793,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -7825,7 +7877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -7857,7 +7909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -7889,7 +7941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -7921,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -7953,7 +8005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -7985,7 +8037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -8017,7 +8069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -8049,7 +8101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -8081,7 +8133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -8113,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -8145,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -8177,7 +8229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -8209,7 +8261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -8241,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -8273,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -8305,7 +8357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -8337,7 +8389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -8369,7 +8421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -8401,7 +8453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -8433,7 +8485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -8465,7 +8517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -8497,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -8529,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -8561,7 +8613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -8593,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -8625,7 +8677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -8657,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -8689,7 +8741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -8721,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -8753,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -8785,7 +8837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -8817,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -8849,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -8881,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -8913,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -8945,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -8977,7 +9029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -9009,7 +9061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -9041,7 +9093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -9073,7 +9125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -9105,7 +9157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -9137,7 +9189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -9169,7 +9221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -9201,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -9233,7 +9285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -9265,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -9297,7 +9349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -9329,7 +9381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -9361,7 +9413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -9393,7 +9445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -9425,7 +9477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -9457,7 +9509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -9489,7 +9541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -9521,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -9553,7 +9605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -9585,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -9617,7 +9669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -9649,7 +9701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -9681,7 +9733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -9713,7 +9765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -9745,7 +9797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -9777,7 +9829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -9809,7 +9861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -9841,7 +9893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -9873,7 +9925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -9905,7 +9957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -9937,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -9969,7 +10021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -10001,7 +10053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>299</v>
       </c>

</xml_diff>